<commit_message>
added more tables to the data
</commit_message>
<xml_diff>
--- a/data/database_tables.xlsx
+++ b/data/database_tables.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17328\Documents\UMBC\CMSC\CMSC_447\CSCoursePlanner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBA436A-D8DB-4AE6-8EA7-C48BA1E1FEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475CF39D-AAEE-4DEC-B537-E256BD7B85B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5C2EA4F3-3AE1-4465-A3C2-3E3AE89E79F6}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="1" xr2:uid="{5C2EA4F3-3AE1-4465-A3C2-3E3AE89E79F6}"/>
   </bookViews>
   <sheets>
     <sheet name="course" sheetId="2" r:id="rId1"/>
-    <sheet name="prereq" sheetId="5" r:id="rId2"/>
-    <sheet name="subject" sheetId="3" r:id="rId3"/>
-    <sheet name="semester" sheetId="1" r:id="rId4"/>
-    <sheet name="major" sheetId="4" r:id="rId5"/>
+    <sheet name="course_offered" sheetId="8" r:id="rId2"/>
+    <sheet name="prereq" sheetId="5" r:id="rId3"/>
+    <sheet name="subject" sheetId="3" r:id="rId4"/>
+    <sheet name="semester" sheetId="1" r:id="rId5"/>
+    <sheet name="major" sheetId="4" r:id="rId6"/>
+    <sheet name="track_requirement" sheetId="9" r:id="rId7"/>
+    <sheet name="gep_requirement" sheetId="7" r:id="rId8"/>
+    <sheet name="degree_requirement" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
   <si>
     <t>semester_id</t>
   </si>
@@ -280,6 +284,27 @@
   </si>
   <si>
     <t>[2, 31]</t>
+  </si>
+  <si>
+    <t>requirement_id</t>
+  </si>
+  <si>
+    <t>requirement_type</t>
+  </si>
+  <si>
+    <t>course_id_options</t>
+  </si>
+  <si>
+    <t>gep_requirement_id</t>
+  </si>
+  <si>
+    <t>gep_type</t>
+  </si>
+  <si>
+    <t>frequency_id</t>
+  </si>
+  <si>
+    <t>offered_prob</t>
   </si>
 </sst>
 </file>
@@ -634,14 +659,14 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="A28" sqref="A28:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.76953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1196,17 +1221,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D31-4266-40C1-848A-2328E59FDBBC}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.58984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFE7A6E-F952-47A2-BF5B-46EDE58757E8}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.75">
@@ -1298,7 +1359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7598D0-838B-4AA9-A52C-CFE2D4CFEB6B}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1308,7 +1369,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="18.953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.75">
@@ -1437,7 +1498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B778B8C-6911-41CE-A0E0-4B4AE2D668B1}">
   <dimension ref="A1:C50"/>
   <sheetViews>
@@ -2002,7 +2063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D41301-DA54-47C4-BC70-4F74F2B7033E}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2012,7 +2073,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="18.953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.75">
@@ -2051,4 +2112,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAF4D59-BF92-4E51-9F3F-C65D5D23AB73}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C73D4EF-9694-4F73-8510-03A47626F400}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E91E79-D5FF-4726-ACE4-F70CEE02F241}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.58984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more offered data
</commit_message>
<xml_diff>
--- a/data/database_tables.xlsx
+++ b/data/database_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17328\Documents\UMBC\CMSC\CMSC_447\CSCoursePlanner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3E0523-3046-4C5F-8F8D-F0EA3E9B468D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B0CB77-4F62-4DDE-9DAD-6A14116F6EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="-40" windowWidth="19280" windowHeight="10160" xr2:uid="{5C2EA4F3-3AE1-4465-A3C2-3E3AE89E79F6}"/>
+    <workbookView xWindow="5" yWindow="5" windowWidth="19190" windowHeight="10070" xr2:uid="{5C2EA4F3-3AE1-4465-A3C2-3E3AE89E79F6}"/>
   </bookViews>
   <sheets>
     <sheet name="course_offered" sheetId="8" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="96">
   <si>
     <t>semester_id</t>
   </si>
@@ -694,21 +694,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D31-4266-40C1-848A-2328E59FDBBC}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
@@ -728,7 +728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -748,7 +748,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -768,7 +768,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3</v>
       </c>
@@ -788,7 +788,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>4</v>
       </c>
@@ -808,7 +808,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>
@@ -828,7 +828,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>6</v>
       </c>
@@ -848,7 +848,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>7</v>
       </c>
@@ -868,7 +868,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>8</v>
       </c>
@@ -888,7 +888,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>9</v>
       </c>
@@ -908,7 +908,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>10</v>
       </c>
@@ -928,7 +928,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>11</v>
       </c>
@@ -948,7 +948,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>12</v>
       </c>
@@ -968,7 +968,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>13</v>
       </c>
@@ -988,7 +988,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1986,6 +1986,26 @@
       </c>
       <c r="F64">
         <v>2023</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>
@@ -2000,7 +2020,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2014,14 +2034,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -2045,9 +2065,9 @@
       <selection activeCell="A2" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2058,7 +2078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2069,7 +2089,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2080,7 +2100,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2091,7 +2111,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2102,7 +2122,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2113,7 +2133,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2124,7 +2144,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2135,7 +2155,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2146,7 +2166,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2157,7 +2177,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2168,7 +2188,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2179,7 +2199,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2190,7 +2210,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2201,7 +2221,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2212,7 +2232,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2223,7 +2243,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2234,7 +2254,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2245,7 +2265,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2256,7 +2276,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2267,7 +2287,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2278,7 +2298,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2289,7 +2309,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2300,7 +2320,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2311,7 +2331,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2322,7 +2342,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2333,7 +2353,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2344,7 +2364,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2355,7 +2375,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2366,7 +2386,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2377,7 +2397,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2388,7 +2408,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2399,7 +2419,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2410,7 +2430,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2421,7 +2441,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2432,7 +2452,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2443,7 +2463,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2454,7 +2474,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2465,7 +2485,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2476,7 +2496,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2487,7 +2507,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2498,7 +2518,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2509,7 +2529,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2520,7 +2540,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2531,7 +2551,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2542,7 +2562,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2553,7 +2573,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2564,7 +2584,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2575,7 +2595,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2586,7 +2606,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2610,12 +2630,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -2626,7 +2646,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2637,7 +2657,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2661,13 +2681,13 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.40625" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -2678,7 +2698,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2689,7 +2709,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2700,7 +2720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2711,7 +2731,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2722,7 +2742,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2733,7 +2753,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2744,7 +2764,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2755,7 +2775,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2766,7 +2786,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2777,7 +2797,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2801,15 +2821,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2826,7 +2846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2843,7 +2863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2860,7 +2880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2877,7 +2897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2894,7 +2914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2911,7 +2931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2928,7 +2948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2945,7 +2965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2962,7 +2982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2979,7 +2999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2996,7 +3016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3013,7 +3033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3030,7 +3050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3047,7 +3067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3064,7 +3084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3081,7 +3101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3098,7 +3118,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3115,7 +3135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3132,7 +3152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3149,7 +3169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3166,7 +3186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3183,7 +3203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3200,7 +3220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3217,7 +3237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3234,7 +3254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3251,7 +3271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3268,7 +3288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3285,7 +3305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3302,7 +3322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3319,7 +3339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3336,7 +3356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3367,15 +3387,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -3402,14 +3422,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.40625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -3439,13 +3459,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.40625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -3456,7 +3476,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3464,7 +3484,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3485,14 +3505,14 @@
       <selection activeCell="D6" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3506,7 +3526,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3520,7 +3540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3534,7 +3554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3548,7 +3568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3562,7 +3582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
added endpoints for courses
</commit_message>
<xml_diff>
--- a/data/database_tables.xlsx
+++ b/data/database_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17328\Documents\UMBC\CMSC\CMSC_447\CSCoursePlanner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B0CB77-4F62-4DDE-9DAD-6A14116F6EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D266F08-B81F-49DA-91D6-D681394C3241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5" yWindow="5" windowWidth="19190" windowHeight="10070" xr2:uid="{5C2EA4F3-3AE1-4465-A3C2-3E3AE89E79F6}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="4" xr2:uid="{5C2EA4F3-3AE1-4465-A3C2-3E3AE89E79F6}"/>
   </bookViews>
   <sheets>
     <sheet name="course_offered" sheetId="8" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="99">
   <si>
     <t>semester_id</t>
   </si>
@@ -334,6 +334,15 @@
   </si>
   <si>
     <t>[]</t>
+  </si>
+  <si>
+    <t>Principles of Digital Design</t>
+  </si>
+  <si>
+    <t>Systems Design and Programming</t>
+  </si>
+  <si>
+    <t>Probability, Statistics, and Random Processes</t>
   </si>
 </sst>
 </file>
@@ -696,19 +705,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D31-4266-40C1-848A-2328E59FDBBC}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
@@ -728,7 +737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -748,7 +757,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -768,7 +777,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -788,7 +797,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -808,7 +817,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -828,7 +837,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -848,7 +857,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -868,7 +877,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -888,7 +897,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -908,7 +917,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -928,7 +937,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -948,7 +957,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -968,7 +977,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -988,7 +997,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1008,7 +1017,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1028,7 +1037,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1048,7 +1057,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1068,7 +1077,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1088,7 +1097,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1108,7 +1117,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1128,7 +1137,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1168,7 +1177,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1188,7 +1197,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1208,7 +1217,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1228,7 +1237,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1268,7 +1277,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1288,7 +1297,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1308,7 +1317,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1328,7 +1337,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1348,7 +1357,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1368,7 +1377,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1388,7 +1397,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1408,7 +1417,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1428,7 +1437,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1448,7 +1457,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1468,7 +1477,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1488,7 +1497,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1508,7 +1517,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1548,7 +1557,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1588,7 +1597,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1608,7 +1617,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1648,7 +1657,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1668,7 +1677,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1688,7 +1697,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1708,7 +1717,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1748,7 +1757,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1768,7 +1777,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1808,7 +1817,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1828,7 +1837,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1848,7 +1857,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1868,7 +1877,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1908,7 +1917,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1948,7 +1957,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1968,7 +1977,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1988,7 +1997,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2020,7 +2029,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2034,14 +2043,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -2065,9 +2074,9 @@
       <selection activeCell="A2" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2078,7 +2087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2089,7 +2098,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2100,7 +2109,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2111,7 +2120,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2122,7 +2131,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2144,7 +2153,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2155,7 +2164,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2177,7 +2186,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2188,7 +2197,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2199,7 +2208,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2210,7 +2219,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2221,7 +2230,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2232,7 +2241,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2243,7 +2252,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2254,7 +2263,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2265,7 +2274,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2276,7 +2285,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2287,7 +2296,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2298,7 +2307,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2309,7 +2318,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2320,7 +2329,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2331,7 +2340,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2342,7 +2351,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2353,7 +2362,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2364,7 +2373,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2375,7 +2384,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2386,7 +2395,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2397,7 +2406,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2408,7 +2417,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2419,7 +2428,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2430,7 +2439,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2441,7 +2450,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2452,7 +2461,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2463,7 +2472,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2474,7 +2483,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2485,7 +2494,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2496,7 +2505,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2507,7 +2516,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2518,7 +2527,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2529,7 +2538,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2540,7 +2549,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2551,7 +2560,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2562,7 +2571,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2573,7 +2582,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2584,7 +2593,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2595,7 +2604,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2606,7 +2615,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2630,12 +2639,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -2646,7 +2655,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2657,7 +2666,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2681,13 +2690,13 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.40625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2709,7 +2718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2720,7 +2729,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2731,7 +2740,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2742,7 +2751,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2753,7 +2762,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2764,7 +2773,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2775,7 +2784,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2786,7 +2795,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2797,7 +2806,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2815,21 +2824,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A7AA6A-156B-4415-998B-9D4BEF27889E}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2846,7 +2855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2863,7 +2872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2880,7 +2889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2897,7 +2906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2914,7 +2923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2931,7 +2940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2948,7 +2957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2965,7 +2974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2982,7 +2991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2999,7 +3008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3016,7 +3025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3033,7 +3042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3050,7 +3059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3067,7 +3076,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3084,7 +3093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3101,7 +3110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3118,7 +3127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3135,7 +3144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3152,7 +3161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3169,7 +3178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3186,7 +3195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3203,7 +3212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3220,7 +3229,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3237,7 +3246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3254,7 +3263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3271,7 +3280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3288,7 +3297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3305,7 +3314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3322,7 +3331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3339,7 +3348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3356,7 +3365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3371,6 +3380,74 @@
       </c>
       <c r="E32">
         <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33">
+        <v>212</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34">
+        <v>310</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35">
+        <v>320</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36">
+        <v>355</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3387,15 +3464,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -3422,14 +3499,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.40625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -3459,13 +3536,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.40625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -3476,7 +3553,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3484,7 +3561,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3505,14 +3582,14 @@
       <selection activeCell="D6" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3526,7 +3603,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3540,7 +3617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3554,7 +3631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3568,7 +3645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3582,7 +3659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
fixed the datascraping script and added data
</commit_message>
<xml_diff>
--- a/data/database_tables.xlsx
+++ b/data/database_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17328\Documents\UMBC\CMSC\CMSC_447\CSCoursePlanner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CE5541-2F51-4F06-BA25-24B23769C61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4AAF85-2F48-40C6-A126-22AA6B2B0C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{5C2EA4F3-3AE1-4465-A3C2-3E3AE89E79F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5C2EA4F3-3AE1-4465-A3C2-3E3AE89E79F6}"/>
   </bookViews>
   <sheets>
     <sheet name="course_offered" sheetId="8" r:id="rId1"/>
@@ -2247,11 +2247,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B778B8C-6911-41CE-A0E0-4B4AE2D668B1}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3003,7 +3006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A7AA6A-156B-4415-998B-9D4BEF27889E}">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>

</xml_diff>